<commit_message>
Work on budget and time plan
</commit_message>
<xml_diff>
--- a/Project Budget.xlsx
+++ b/Project Budget.xlsx
@@ -2,7 +2,6 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="14220" windowHeight="8580"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="14220" windowHeight="8580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Project:</t>
   </si>
@@ -113,15 +112,17 @@
   </si>
   <si>
     <t>Backend programming for Assessment Designer</t>
+  </si>
+  <si>
+    <t>Semester 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -235,16 +236,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -645,28 +646,33 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
     <col min="7" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="2.28515625" customWidth="1"/>
+    <col min="9" max="9" width="2.33203125" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -674,7 +680,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -682,7 +688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -690,21 +696,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -715,13 +721,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>8</v>
       </c>
@@ -732,7 +738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>1</v>
       </c>
@@ -748,7 +754,7 @@
         <v>15.25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>2</v>
       </c>
@@ -764,7 +770,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>3</v>
       </c>
@@ -780,7 +786,7 @@
         <v>114.375</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>4</v>
       </c>
@@ -789,14 +795,14 @@
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="9">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E16" s="10">
         <f t="shared" ref="E16:E20" si="0">D16*$D$9</f>
-        <v>106.75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+        <v>198.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>5</v>
       </c>
@@ -805,14 +811,14 @@
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="9">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E17" s="10">
         <f t="shared" si="0"/>
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+        <v>503.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>6</v>
       </c>
@@ -821,14 +827,14 @@
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="9">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E18" s="10">
         <f t="shared" si="0"/>
-        <v>244</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>7</v>
       </c>
@@ -837,14 +843,14 @@
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="9">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E19" s="10">
         <f t="shared" si="0"/>
-        <v>533.75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>10</v>
       </c>
@@ -853,14 +859,14 @@
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="9">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E20" s="10">
         <f t="shared" si="0"/>
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>11</v>
       </c>
@@ -874,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>12</v>
       </c>
@@ -888,13 +894,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
     </row>
-    <row r="24" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>13</v>
       </c>
@@ -902,22 +908,22 @@
       <c r="C24" s="14"/>
       <c r="D24" s="9">
         <f>SUM(D13:D23)</f>
-        <v>90.5</v>
+        <v>138.5</v>
       </c>
       <c r="E24" s="19">
         <f>SUM(E13:E23)</f>
-        <v>1380.125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+        <v>2112.125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>16</v>
       </c>
@@ -928,7 +934,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>18</v>
       </c>
@@ -936,36 +942,36 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="21">
         <f>(E24)+(E24)*C28</f>
-        <v>2070.1875</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3168.1875</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>20</v>
       </c>
       <c r="C32" s="21">
         <f>C31*C29</f>
-        <v>828.07500000000005</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+        <v>1267.2750000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>21</v>
       </c>
       <c r="C33" s="21">
         <f>C32+C31</f>
-        <v>2898.2624999999998</v>
+        <v>4435.4624999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final draft of Project Proposal
</commit_message>
<xml_diff>
--- a/Project Budget.xlsx
+++ b/Project Budget.xlsx
@@ -33,9 +33,6 @@
     <t>EXPENDITURE</t>
   </si>
   <si>
-    <t>A: SALARY</t>
-  </si>
-  <si>
     <t>Design charge rate:</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Client meetings</t>
   </si>
   <si>
-    <t>C: FINAL QUOTE  &amp; PROFIT / (LOSS)</t>
-  </si>
-  <si>
     <t>Overhead allowance:</t>
   </si>
   <si>
@@ -115,6 +109,12 @@
   </si>
   <si>
     <t>Semester 1</t>
+  </si>
+  <si>
+    <t>SALARY</t>
+  </si>
+  <si>
+    <t>FINAL QUOTE  &amp; PROFIT / (LOSS)</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -664,12 +664,12 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -693,7 +693,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -707,35 +707,35 @@
     </row>
     <row r="8" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="3">
         <v>15.25</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -743,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="7">
@@ -759,7 +759,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="17">
@@ -775,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="9">
@@ -791,7 +791,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="9">
@@ -807,7 +807,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="9">
@@ -823,7 +823,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="9">
@@ -839,7 +839,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="9">
@@ -855,7 +855,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="9">
@@ -871,7 +871,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="9"/>
@@ -885,7 +885,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="9"/>
@@ -923,12 +923,15 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
     </row>
+    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
-        <v>16</v>
-      </c>
+      <c r="A28" s="18"/>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28" s="20">
         <v>0.5</v>
@@ -936,7 +939,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C29" s="20">
         <v>0.4</v>
@@ -944,12 +947,12 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C31" s="21">
         <f>(E24)+(E24)*C28</f>
@@ -958,7 +961,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C32" s="21">
         <f>C31*C29</f>
@@ -967,7 +970,7 @@
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C33" s="21">
         <f>C32+C31</f>

</xml_diff>